<commit_message>
chasing qpsk TX distort
</commit_message>
<xml_diff>
--- a/PSK_test.xlsx
+++ b/PSK_test.xlsx
@@ -396,7 +396,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -476,15 +476,15 @@
         <v>5</v>
       </c>
       <c r="D4" s="1">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E4" s="1">
         <f>D4*0.12</f>
-        <v>8.16</v>
+        <v>8.2799999999999994</v>
       </c>
       <c r="F4" s="1">
         <f>E4-E3</f>
-        <v>3.4800000000000004</v>
+        <v>3.5999999999999996</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -506,7 +506,7 @@
       </c>
       <c r="F5" s="1">
         <f>E5-E4</f>
-        <v>4.92</v>
+        <v>4.8000000000000007</v>
       </c>
     </row>
     <row r="10" spans="1:6">

</xml_diff>

<commit_message>
C25 RRC pulse table scale
</commit_message>
<xml_diff>
--- a/PSK_test.xlsx
+++ b/PSK_test.xlsx
@@ -1,18 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninocarrillo/github/N9600A-sim/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A31AA0-CAEE-2443-AD7F-A2FD16DF234C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="10515" windowHeight="9540"/>
+    <workbookView xWindow="4480" yWindow="2220" windowWidth="17200" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -61,8 +79,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,13 +123,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -149,7 +175,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -183,6 +209,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -217,9 +244,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -392,23 +420,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="10.5703125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.1640625" style="1"/>
+    <col min="5" max="5" width="10.5" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="60">
+    <row r="1" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -425,7 +453,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>300</v>
       </c>
@@ -443,7 +471,7 @@
         <v>2.16</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>300</v>
       </c>
@@ -465,7 +493,7 @@
         <v>2.5199999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>300</v>
       </c>
@@ -476,18 +504,18 @@
         <v>5</v>
       </c>
       <c r="D4" s="1">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="E4" s="1">
         <f>D4*0.12</f>
-        <v>8.2799999999999994</v>
+        <v>9</v>
       </c>
       <c r="F4" s="1">
         <f>E4-E3</f>
-        <v>3.5999999999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>4.32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>300</v>
       </c>
@@ -506,10 +534,10 @@
       </c>
       <c r="F5" s="1">
         <f>E5-E4</f>
-        <v>4.8000000000000007</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>4.08</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -517,25 +545,25 @@
         <v>229</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="1">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="1">
         <f>14400*C11*C10/(32768*65536)</f>
-        <v>30.71129322052002</v>
+        <v>46.066939830780029</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:E5">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E5">
     <sortCondition ref="D2:D5"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -544,24 +572,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
m26 beta to Tom/Mitch
</commit_message>
<xml_diff>
--- a/PSK_test.xlsx
+++ b/PSK_test.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninocarrillo/github/N9600A-sim/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED0D3E7-D429-9546-BEFD-F62BCAA5F6B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10080" yWindow="1875" windowWidth="10515" windowHeight="9540" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="10080" yWindow="1880" windowWidth="10520" windowHeight="9540" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Span 6 RRC 0.495" sheetId="1" r:id="rId1"/>
@@ -12,7 +18,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Span 6 RRC 0.6 Tukey" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -110,8 +116,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,9 +172,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -206,7 +212,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -240,6 +246,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -274,9 +281,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -449,24 +457,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="60">
+    <row r="1" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,7 +494,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>300</v>
       </c>
@@ -504,7 +512,7 @@
         <v>2.16</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>300</v>
       </c>
@@ -526,7 +534,7 @@
         <v>2.5199999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>300</v>
       </c>
@@ -551,7 +559,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>300</v>
       </c>
@@ -573,7 +581,7 @@
         <v>4.9199999999999982</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
@@ -582,7 +590,7 @@
         <v>9.7199999999999989</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
@@ -591,7 +599,7 @@
         <v>4.8000000000000007</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -599,7 +607,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
@@ -607,7 +615,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
@@ -617,7 +625,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:E5">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E5">
     <sortCondition ref="D2:D5"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -626,48 +634,48 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="11.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="60">
+    <row r="1" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -684,7 +692,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>300</v>
       </c>
@@ -699,7 +707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>300</v>
       </c>
@@ -717,7 +725,7 @@
         <v>1.68</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>300</v>
       </c>
@@ -728,14 +736,14 @@
         <v>5</v>
       </c>
       <c r="D4" s="1">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>4.68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>4.4399999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>300</v>
       </c>
@@ -759,7 +767,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1200</v>
       </c>
@@ -783,7 +791,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1200</v>
       </c>
@@ -805,7 +813,7 @@
         <v>6.8124123737558717</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>2400</v>
       </c>
@@ -823,22 +831,22 @@
         <v>3.5999999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E10" s="1">
         <f>E5-E3</f>
         <v>6.3599999999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="1">
         <f>E4-E3</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+        <v>2.76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D12" s="1" t="s">
         <v>16</v>
       </c>
@@ -847,7 +855,7 @@
         <v>0.23999999999999932</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
@@ -855,7 +863,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
@@ -863,7 +871,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
@@ -872,7 +880,7 @@
         <v>108.7971031665802</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
@@ -880,7 +888,7 @@
         <v>7100</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>18</v>
       </c>
@@ -888,7 +896,7 @@
         <v>65536</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
@@ -896,7 +904,7 @@
         <v>14400</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
@@ -904,7 +912,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
@@ -913,7 +921,7 @@
         <v>1560.05859375</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
n26 adjust QPSK 2400 integral limit
</commit_message>
<xml_diff>
--- a/PSK_test.xlsx
+++ b/PSK_test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninocarrillo/github/N9600A-sim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED0D3E7-D429-9546-BEFD-F62BCAA5F6B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0C61D5-24AA-F543-B0A5-9921EC01BBC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10080" yWindow="1880" windowWidth="10520" windowHeight="9540" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>Baud</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Wide</t>
+  </si>
+  <si>
+    <t>Perfect 100</t>
   </si>
 </sst>
 </file>
@@ -662,7 +665,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -691,6 +694,9 @@
       <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
@@ -742,6 +748,9 @@
         <f t="shared" si="0"/>
         <v>4.4399999999999995</v>
       </c>
+      <c r="F4" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -760,6 +769,9 @@
         <f t="shared" si="0"/>
         <v>8.0399999999999991</v>
       </c>
+      <c r="F5" s="1">
+        <v>100</v>
+      </c>
       <c r="G5" s="1" t="s">
         <v>23</v>
       </c>
@@ -784,6 +796,9 @@
         <f t="shared" si="0"/>
         <v>7.8</v>
       </c>
+      <c r="F6" s="1">
+        <v>100</v>
+      </c>
       <c r="G6" s="1" t="s">
         <v>24</v>
       </c>
@@ -815,7 +830,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>2400</v>
+        <v>1200</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>7</v>
@@ -824,11 +839,14 @@
         <v>5</v>
       </c>
       <c r="D8" s="1">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>3.5999999999999996</v>
+        <v>3.84</v>
+      </c>
+      <c r="F8" s="1">
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>